<commit_message>
Added data for May and June
</commit_message>
<xml_diff>
--- a/src/rte_trend_data.xlsx
+++ b/src/rte_trend_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,9 @@
         <v>0</v>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -501,7 +503,9 @@
         <v>0</v>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -516,7 +520,9 @@
         <v>770</v>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -531,7 +537,9 @@
         <v>1093</v>
       </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -546,7 +554,9 @@
         <v>242</v>
       </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -559,7 +569,9 @@
         <v>0</v>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -572,7 +584,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -585,7 +599,9 @@
         <v>0</v>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -598,7 +614,9 @@
         <v>0</v>
       </c>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>0.832</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -631,6 +649,40 @@
         <v>0.867</v>
       </c>
       <c r="E13" t="n">
+        <v>0.832</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.8023110536204735</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>0.832</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8902329256087044</v>
+      </c>
+      <c r="C15" t="n">
+        <v>97</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
         <v>0.832</v>
       </c>
     </row>

</xml_diff>